<commit_message>
GPP to Science Param Editor
Added GPP to Science Param Editor; Fixed typo (missing }) in Missing History Config;
</commit_message>
<xml_diff>
--- a/Source/Science.xlsx
+++ b/Source/Science.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEA3259-39C9-4AD2-B1FD-AF5358CB970E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C8D594-78DD-425B-8C7E-391AF0542FB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11230" windowWidth="12800" windowHeight="9200" activeTab="1" xr2:uid="{18B22CFD-9E2F-4ACB-8B6C-C8C8B7035FA5}"/>
+    <workbookView xWindow="820" yWindow="730" windowWidth="17390" windowHeight="19090" activeTab="2" xr2:uid="{18B22CFD-9E2F-4ACB-8B6C-C8C8B7035FA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Defaults!$A$1:$D$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kiwi!$A$2:$X$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ScienceParam!$A$1:$M$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stock!$A$2:$U$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="247">
   <si>
     <t>Experiment</t>
   </si>
@@ -687,6 +688,102 @@
   </si>
   <si>
     <t>!EXPERIMENT_DEFINITION:HAS[#id[photo-*]:NEEDS[FeatureScience]</t>
+  </si>
+  <si>
+    <t>Icarus</t>
+  </si>
+  <si>
+    <t>GPP</t>
+  </si>
+  <si>
+    <t>Thalia</t>
+  </si>
+  <si>
+    <t>Eta</t>
+  </si>
+  <si>
+    <t>Niven</t>
+  </si>
+  <si>
+    <t>Squad,!GPP</t>
+  </si>
+  <si>
+    <t>Gael</t>
+  </si>
+  <si>
+    <t>Iota</t>
+  </si>
+  <si>
+    <t>Ceti</t>
+  </si>
+  <si>
+    <t>Tellumo</t>
+  </si>
+  <si>
+    <t>Lili</t>
+  </si>
+  <si>
+    <t>Gratian</t>
+  </si>
+  <si>
+    <t>Geminus</t>
+  </si>
+  <si>
+    <t>Otho</t>
+  </si>
+  <si>
+    <t>Augustus</t>
+  </si>
+  <si>
+    <t>Hephaestus</t>
+  </si>
+  <si>
+    <t>Jannah</t>
+  </si>
+  <si>
+    <t>Gauss</t>
+  </si>
+  <si>
+    <t>Loki</t>
+  </si>
+  <si>
+    <t>Catullus</t>
+  </si>
+  <si>
+    <t>Tarsiss</t>
+  </si>
+  <si>
+    <t>Nero</t>
+  </si>
+  <si>
+    <t>Hadrian</t>
+  </si>
+  <si>
+    <t>Narisse</t>
+  </si>
+  <si>
+    <t>Muse</t>
+  </si>
+  <si>
+    <t>Minona</t>
+  </si>
+  <si>
+    <t>Agrippina</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Hox</t>
+  </si>
+  <si>
+    <t>Argo</t>
+  </si>
+  <si>
+    <t>Leto</t>
+  </si>
+  <si>
+    <t>GEP|GPP</t>
   </si>
 </sst>
 </file>
@@ -4326,7 +4423,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -11550,13 +11647,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F6E689-7182-4BC0-80F9-0B8DE28A1A46}">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11646,8 +11741,8 @@
         <v>1000000000</v>
       </c>
       <c r="M2" s="1" t="str">
-        <f>_xlfn.CONCAT("Item",CHAR(10),"{",CHAR(10),"    bodyName = ",A2,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C2,CHAR(10),"        ",D$1," = ",D2,CHAR(10),"        ",E$1," = ",E2,CHAR(10),"        ",F$1," = ",F2,CHAR(10),"        ",G$1," = ",G2,CHAR(10),"        ",H$1," = ",H2,CHAR(10),"        ",I$1," = ",I2,CHAR(10),"        ",J$1," = ",J2,CHAR(10),"        ",K$1," = ",K2,CHAR(10),"    }",CHAR(10),"}")</f>
-        <v>Item
+        <f>_xlfn.CONCAT("Item:NEEDS[",B2,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A2,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C2,CHAR(10),"        ",D$1," = ",D2,CHAR(10),"        ",E$1," = ",E2,CHAR(10),"        ",F$1," = ",F2,CHAR(10),"        ",G$1," = ",G2,CHAR(10),"        ",H$1," = ",H2,CHAR(10),"        ",I$1," = ",I2,CHAR(10),"        ",J$1," = ",J2,CHAR(10),"        ",K$1," = ",K2,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Sun
     adjustedParams
@@ -11670,7 +11765,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>220</v>
       </c>
       <c r="C3">
         <v>0.8</v>
@@ -11700,8 +11795,8 @@
         <v>250000</v>
       </c>
       <c r="M3" s="1" t="str">
-        <f t="shared" ref="M3:M63" si="0">_xlfn.CONCAT("Item",CHAR(10),"{",CHAR(10),"    bodyName = ",A3,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C3,CHAR(10),"        ",D$1," = ",D3,CHAR(10),"        ",E$1," = ",E3,CHAR(10),"        ",F$1," = ",F3,CHAR(10),"        ",G$1," = ",G3,CHAR(10),"        ",H$1," = ",H3,CHAR(10),"        ",I$1," = ",I3,CHAR(10),"        ",J$1," = ",J3,CHAR(10),"        ",K$1," = ",K3,CHAR(10),"    }",CHAR(10),"}")</f>
-        <v>Item
+        <f t="shared" ref="M3:M66" si="0">_xlfn.CONCAT("Item:NEEDS[",B3,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A3,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C3,CHAR(10),"        ",D$1," = ",D3,CHAR(10),"        ",E$1," = ",E3,CHAR(10),"        ",F$1," = ",F3,CHAR(10),"        ",G$1," = ",G3,CHAR(10),"        ",H$1," = ",H3,CHAR(10),"        ",I$1," = ",I3,CHAR(10),"        ",J$1," = ",J3,CHAR(10),"        ",K$1," = ",K3,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[Squad,!GPP]
 {
     bodyName = Kerbin
     adjustedParams
@@ -11738,7 +11833,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:H62" si="1">$C4-1</f>
+        <f t="shared" ref="F4:H67" si="1">$C4-1</f>
         <v>2</v>
       </c>
       <c r="G4">
@@ -11760,7 +11855,7 @@
       </c>
       <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Mun
     adjustedParams
@@ -11789,11 +11884,11 @@
         <v>3.5</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D62" si="2">$C5</f>
+        <f t="shared" ref="D5:D67" si="2">$C5</f>
         <v>3.5</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E62" si="3">$C5-1</f>
+        <f t="shared" ref="E5:E67" si="3">$C5-1</f>
         <v>2.5</v>
       </c>
       <c r="F5">
@@ -11819,7 +11914,7 @@
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Minmus
     adjustedParams
@@ -11878,7 +11973,7 @@
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Moho
     adjustedParams
@@ -11937,7 +12032,7 @@
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Eve
     adjustedParams
@@ -11996,7 +12091,7 @@
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Duna
     adjustedParams
@@ -12055,7 +12150,7 @@
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Ike
     adjustedParams
@@ -12114,7 +12209,7 @@
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Jool
     adjustedParams
@@ -12173,7 +12268,7 @@
       </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Laythe
     adjustedParams
@@ -12232,7 +12327,7 @@
       </c>
       <c r="M12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Vall
     adjustedParams
@@ -12291,7 +12386,7 @@
       </c>
       <c r="M13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Bop
     adjustedParams
@@ -12350,7 +12445,7 @@
       </c>
       <c r="M14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Tylo
     adjustedParams
@@ -12409,7 +12504,7 @@
       </c>
       <c r="M15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Gilly
     adjustedParams
@@ -12468,7 +12563,7 @@
       </c>
       <c r="M16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Pol
     adjustedParams
@@ -12527,7 +12622,7 @@
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Dres
     adjustedParams
@@ -12586,7 +12681,7 @@
       </c>
       <c r="M18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[Squad]
 {
     bodyName = Eeloo
     adjustedParams
@@ -12648,7 +12743,7 @@
       </c>
       <c r="M19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Nissee
     adjustedParams
@@ -12710,7 +12805,7 @@
       </c>
       <c r="M20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Thatmo
     adjustedParams
@@ -12772,7 +12867,7 @@
       </c>
       <c r="M21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Karen
     adjustedParams
@@ -12834,7 +12929,7 @@
       </c>
       <c r="M22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Tekto
     adjustedParams
@@ -12896,7 +12991,7 @@
       </c>
       <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Slate
     adjustedParams
@@ -12958,7 +13053,7 @@
       </c>
       <c r="M24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Ovok
     adjustedParams
@@ -13020,7 +13115,7 @@
       </c>
       <c r="M25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Hale
     adjustedParams
@@ -13082,7 +13177,7 @@
       </c>
       <c r="M26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Wal
     adjustedParams
@@ -13144,7 +13239,7 @@
       </c>
       <c r="M27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Tal
     adjustedParams
@@ -13206,7 +13301,7 @@
       </c>
       <c r="M28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Priax
     adjustedParams
@@ -13268,7 +13363,7 @@
       </c>
       <c r="M29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Polta
     adjustedParams
@@ -13330,7 +13425,7 @@
       </c>
       <c r="M30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Urlum
     adjustedParams
@@ -13392,7 +13487,7 @@
       </c>
       <c r="M31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Sarnus
     adjustedParams
@@ -13454,7 +13549,7 @@
       </c>
       <c r="M32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Plock
     adjustedParams
@@ -13516,7 +13611,7 @@
       </c>
       <c r="M33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[OPM]
 {
     bodyName = Neidon
     adjustedParams
@@ -13578,7 +13673,7 @@
       </c>
       <c r="M34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Ki'Ki
     adjustedParams
@@ -13640,7 +13735,7 @@
       </c>
       <c r="M35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Kal
     adjustedParams
@@ -13702,7 +13797,7 @@
       </c>
       <c r="M36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Havous
     adjustedParams
@@ -13764,7 +13859,7 @@
       </c>
       <c r="M37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Geito
     adjustedParams
@@ -13826,7 +13921,7 @@
       </c>
       <c r="M38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Archae
     adjustedParams
@@ -13888,7 +13983,7 @@
       </c>
       <c r="M39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Ervo
     adjustedParams
@@ -13950,7 +14045,7 @@
       </c>
       <c r="M40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Edas
     adjustedParams
@@ -14012,7 +14107,7 @@
       </c>
       <c r="M41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Crokslev
     adjustedParams
@@ -14074,7 +14169,7 @@
       </c>
       <c r="M42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Zore
     adjustedParams
@@ -14136,7 +14231,7 @@
       </c>
       <c r="M43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Vant
     adjustedParams
@@ -14198,7 +14293,7 @@
       </c>
       <c r="M44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Lon
     adjustedParams
@@ -14260,7 +14355,7 @@
       </c>
       <c r="M45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Soden
     adjustedParams
@@ -14322,7 +14417,7 @@
       </c>
       <c r="M46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Flake
     adjustedParams
@@ -14384,7 +14479,7 @@
       </c>
       <c r="M47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Mracksis
     adjustedParams
@@ -14446,7 +14541,7 @@
       </c>
       <c r="M48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[MPE]
 {
     bodyName = Lint-Mikey
     adjustedParams
@@ -14508,7 +14603,7 @@
       </c>
       <c r="M49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Epona
     adjustedParams
@@ -14570,7 +14665,7 @@
       </c>
       <c r="M50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Damona
     adjustedParams
@@ -14632,7 +14727,7 @@
       </c>
       <c r="M51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Cernunnos
     adjustedParams
@@ -14694,7 +14789,7 @@
       </c>
       <c r="M52" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Caireen
     adjustedParams
@@ -14756,7 +14851,7 @@
       </c>
       <c r="M53" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Brovo
     adjustedParams
@@ -14818,7 +14913,7 @@
       </c>
       <c r="M54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Belisama
     adjustedParams
@@ -14880,7 +14975,7 @@
       </c>
       <c r="M55" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Airmed
     adjustedParams
@@ -14942,7 +15037,7 @@
       </c>
       <c r="M56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Toutatis
     adjustedParams
@@ -15004,7 +15099,7 @@
       </c>
       <c r="M57" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Taranis
     adjustedParams
@@ -15066,7 +15161,7 @@
       </c>
       <c r="M58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Sucellus
     adjustedParams
@@ -15128,7 +15223,7 @@
       </c>
       <c r="M59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Sirona
     adjustedParams
@@ -15190,7 +15285,7 @@
       </c>
       <c r="M60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Rosmerta
     adjustedParams
@@ -15252,7 +15347,7 @@
       </c>
       <c r="M61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = RAB-58E
     adjustedParams
@@ -15314,7 +15409,7 @@
       </c>
       <c r="M62" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP]
 {
     bodyName = Nodens
     adjustedParams
@@ -15337,7 +15432,7 @@
         <v>158</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -15355,7 +15450,7 @@
         <v>20</v>
       </c>
       <c r="H63">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I63">
         <v>25</v>
@@ -15371,7 +15466,7 @@
       </c>
       <c r="M63" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Item
+        <v>Item:NEEDS[GEP|GPP]
 {
     bodyName = Grannus
     adjustedParams
@@ -15381,7 +15476,7 @@
         flyingLowData = 5
         flyingHighData = 5
         spaceLowData = 20
-        spaceHighData = 8
+        spaceHighData = 12
         recoveredData = 25
         flyingThreshold = 200000
         spaceThreshold = 50000000000
@@ -15389,7 +15484,1768 @@
 }</v>
       </c>
     </row>
+    <row r="64" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>215</v>
+      </c>
+      <c r="B64" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>9</v>
+      </c>
+      <c r="J64">
+        <v>18000</v>
+      </c>
+      <c r="K64">
+        <v>80000</v>
+      </c>
+      <c r="M64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Icarus
+    adjustedParams
+    {
+        landedData = 5
+        splashedData = 5
+        flyingLowData = 4
+        flyingHighData = 4
+        spaceLowData = 4
+        spaceHighData = 4
+        recoveredData = 9
+        flyingThreshold = 18000
+        spaceThreshold = 80000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" t="s">
+        <v>216</v>
+      </c>
+      <c r="C65">
+        <v>4.5</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="I65">
+        <v>7</v>
+      </c>
+      <c r="J65">
+        <v>22000</v>
+      </c>
+      <c r="K65">
+        <v>250000</v>
+      </c>
+      <c r="M65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Thalia
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 7
+        flyingThreshold = 22000
+        spaceThreshold = 250000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" t="s">
+        <v>216</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I66">
+        <v>8</v>
+      </c>
+      <c r="J66">
+        <v>18000</v>
+      </c>
+      <c r="K66">
+        <v>30000</v>
+      </c>
+      <c r="M66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Eta
+    adjustedParams
+    {
+        landedData = 4
+        splashedData = 4
+        flyingLowData = 3
+        flyingHighData = 3
+        spaceLowData = 3
+        spaceHighData = 3
+        recoveredData = 8
+        flyingThreshold = 18000
+        spaceThreshold = 30000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67">
+        <v>4.5</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67">
+        <v>16000</v>
+      </c>
+      <c r="K67">
+        <v>200000</v>
+      </c>
+      <c r="M67" s="1" t="str">
+        <f t="shared" ref="M67:M68" si="4">_xlfn.CONCAT("Item:NEEDS[",B67,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A67,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C67,CHAR(10),"        ",D$1," = ",D67,CHAR(10),"        ",E$1," = ",E67,CHAR(10),"        ",F$1," = ",F67,CHAR(10),"        ",G$1," = ",G67,CHAR(10),"        ",H$1," = ",H67,CHAR(10),"        ",I$1," = ",I67,CHAR(10),"        ",J$1," = ",J67,CHAR(10),"        ",K$1," = ",K67,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Niven
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 5
+        flyingThreshold = 16000
+        spaceThreshold = 200000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68">
+        <v>0.8</v>
+      </c>
+      <c r="D68">
+        <v>0.8</v>
+      </c>
+      <c r="E68">
+        <v>0.8</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1.5</v>
+      </c>
+      <c r="H68">
+        <v>1.5</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>18000</v>
+      </c>
+      <c r="K68">
+        <v>300000</v>
+      </c>
+      <c r="M68" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Kerbin
+    adjustedParams
+    {
+        landedData = 0.8
+        splashedData = 0.8
+        flyingLowData = 0.8
+        flyingHighData = 1
+        spaceLowData = 1.5
+        spaceHighData = 1.5
+        recoveredData = 1
+        flyingThreshold = 18000
+        spaceThreshold = 300000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" t="s">
+        <v>216</v>
+      </c>
+      <c r="C69">
+        <v>0.8</v>
+      </c>
+      <c r="D69">
+        <v>0.8</v>
+      </c>
+      <c r="E69">
+        <v>0.8</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>1.5</v>
+      </c>
+      <c r="H69">
+        <v>1.5</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>18000</v>
+      </c>
+      <c r="K69">
+        <v>300000</v>
+      </c>
+      <c r="M69" s="1" t="str">
+        <f t="shared" ref="M69:M73" si="5">_xlfn.CONCAT("Item:NEEDS[",B69,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A69,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C69,CHAR(10),"        ",D$1," = ",D69,CHAR(10),"        ",E$1," = ",E69,CHAR(10),"        ",F$1," = ",F69,CHAR(10),"        ",G$1," = ",G69,CHAR(10),"        ",H$1," = ",H69,CHAR(10),"        ",I$1," = ",I69,CHAR(10),"        ",J$1," = ",J69,CHAR(10),"        ",K$1," = ",K69,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Gael
+    adjustedParams
+    {
+        landedData = 0.8
+        splashedData = 0.8
+        flyingLowData = 0.8
+        flyingHighData = 1
+        spaceLowData = 1.5
+        spaceHighData = 1.5
+        recoveredData = 1
+        flyingThreshold = 18000
+        spaceThreshold = 300000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70">
+        <v>3.5</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ref="D70" si="6">$C70</f>
+        <v>3.5</v>
+      </c>
+      <c r="E70">
+        <f t="shared" ref="E70:H93" si="7">$C70-1</f>
+        <v>2.5</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+      <c r="J70">
+        <v>18000</v>
+      </c>
+      <c r="K70">
+        <v>50000</v>
+      </c>
+      <c r="M70" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Iota
+    adjustedParams
+    {
+        landedData = 3.5
+        splashedData = 3.5
+        flyingLowData = 2.5
+        flyingHighData = 2.5
+        spaceLowData = 2.5
+        spaceHighData = 2.5
+        recoveredData = 2
+        flyingThreshold = 18000
+        spaceThreshold = 50000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <f>$C71</f>
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <f>$C71-1</f>
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+      <c r="J71">
+        <v>18000</v>
+      </c>
+      <c r="K71">
+        <v>75000</v>
+      </c>
+      <c r="M71" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Ceti
+    adjustedParams
+    {
+        landedData = 3
+        splashedData = 3
+        flyingLowData = 2
+        flyingHighData = 2
+        spaceLowData = 2
+        spaceHighData = 2
+        recoveredData = 3
+        flyingThreshold = 18000
+        spaceThreshold = 75000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" t="s">
+        <v>216</v>
+      </c>
+      <c r="C72">
+        <v>4.5</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ref="D72:D93" si="8">$C72</f>
+        <v>4.5</v>
+      </c>
+      <c r="E72">
+        <f t="shared" ref="E72:E93" si="9">$C72-1</f>
+        <v>3.5</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="I72">
+        <v>6</v>
+      </c>
+      <c r="J72">
+        <v>11000</v>
+      </c>
+      <c r="K72">
+        <v>500000</v>
+      </c>
+      <c r="M72" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Tellumo
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 6
+        flyingThreshold = 11000
+        spaceThreshold = 500000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>225</v>
+      </c>
+      <c r="B73" t="s">
+        <v>216</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="I73">
+        <v>7</v>
+      </c>
+      <c r="J73">
+        <v>9000</v>
+      </c>
+      <c r="K73">
+        <v>10000</v>
+      </c>
+      <c r="M73" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Lili
+    adjustedParams
+    {
+        landedData = 4
+        splashedData = 4
+        flyingLowData = 3
+        flyingHighData = 3
+        spaceLowData = 3
+        spaceHighData = 3
+        recoveredData = 7
+        flyingThreshold = 9000
+        spaceThreshold = 10000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" t="s">
+        <v>216</v>
+      </c>
+      <c r="C74">
+        <v>4.5</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="9"/>
+        <v>3.5</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="I74">
+        <v>8</v>
+      </c>
+      <c r="J74">
+        <v>13000</v>
+      </c>
+      <c r="K74">
+        <v>275000</v>
+      </c>
+      <c r="M74" s="1" t="str">
+        <f t="shared" ref="M74:M78" si="10">_xlfn.CONCAT("Item:NEEDS[",B74,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A74,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C74,CHAR(10),"        ",D$1," = ",D74,CHAR(10),"        ",E$1," = ",E74,CHAR(10),"        ",F$1," = ",F74,CHAR(10),"        ",G$1," = ",G74,CHAR(10),"        ",H$1," = ",H74,CHAR(10),"        ",I$1," = ",I74,CHAR(10),"        ",J$1," = ",J74,CHAR(10),"        ",K$1," = ",K74,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Gratian
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 8
+        flyingThreshold = 13000
+        spaceThreshold = 275000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>227</v>
+      </c>
+      <c r="B75" t="s">
+        <v>216</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="I75">
+        <v>9</v>
+      </c>
+      <c r="J75">
+        <v>18000</v>
+      </c>
+      <c r="K75">
+        <v>115000</v>
+      </c>
+      <c r="M75" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Geminus
+    adjustedParams
+    {
+        landedData = 4
+        splashedData = 4
+        flyingLowData = 3
+        flyingHighData = 3
+        spaceLowData = 3
+        spaceHighData = 3
+        recoveredData = 9
+        flyingThreshold = 18000
+        spaceThreshold = 115000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>228</v>
+      </c>
+      <c r="B76" t="s">
+        <v>216</v>
+      </c>
+      <c r="C76">
+        <v>5.5</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="8"/>
+        <v>5.5</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="9"/>
+        <v>4.5</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="I76">
+        <v>10</v>
+      </c>
+      <c r="J76">
+        <v>300000</v>
+      </c>
+      <c r="K76">
+        <v>1750000</v>
+      </c>
+      <c r="M76" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Otho
+    adjustedParams
+    {
+        landedData = 5.5
+        splashedData = 5.5
+        flyingLowData = 4.5
+        flyingHighData = 4.5
+        spaceLowData = 4.5
+        spaceHighData = 4.5
+        recoveredData = 10
+        flyingThreshold = 300000
+        spaceThreshold = 1750000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I77">
+        <v>11</v>
+      </c>
+      <c r="J77">
+        <v>15000</v>
+      </c>
+      <c r="K77">
+        <v>175000</v>
+      </c>
+      <c r="M77" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Augustus
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 11
+        flyingThreshold = 15000
+        spaceThreshold = 175000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>230</v>
+      </c>
+      <c r="B78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78">
+        <v>4.5</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="9"/>
+        <v>3.5</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="I78">
+        <v>11</v>
+      </c>
+      <c r="J78">
+        <v>18000</v>
+      </c>
+      <c r="K78">
+        <v>62500</v>
+      </c>
+      <c r="M78" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Hephaestus
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 11
+        flyingThreshold = 18000
+        spaceThreshold = 62500
+    }
+}</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>231</v>
+      </c>
+      <c r="B79" t="s">
+        <v>216</v>
+      </c>
+      <c r="C79">
+        <v>4.5</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="9"/>
+        <v>3.5</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="I79">
+        <v>11</v>
+      </c>
+      <c r="J79">
+        <v>18000</v>
+      </c>
+      <c r="K79">
+        <v>52500</v>
+      </c>
+      <c r="M79" s="1" t="str">
+        <f t="shared" ref="M79:M81" si="11">_xlfn.CONCAT("Item:NEEDS[",B79,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A79,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C79,CHAR(10),"        ",D$1," = ",D79,CHAR(10),"        ",E$1," = ",E79,CHAR(10),"        ",F$1," = ",F79,CHAR(10),"        ",G$1," = ",G79,CHAR(10),"        ",H$1," = ",H79,CHAR(10),"        ",I$1," = ",I79,CHAR(10),"        ",J$1," = ",J79,CHAR(10),"        ",K$1," = ",K79,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Jannah
+    adjustedParams
+    {
+        landedData = 4.5
+        splashedData = 4.5
+        flyingLowData = 3.5
+        flyingHighData = 3.5
+        spaceLowData = 3.5
+        spaceHighData = 3.5
+        recoveredData = 11
+        flyingThreshold = 18000
+        spaceThreshold = 52500
+    }
+}</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I80">
+        <v>11</v>
+      </c>
+      <c r="J80">
+        <v>200000</v>
+      </c>
+      <c r="K80">
+        <v>1250000</v>
+      </c>
+      <c r="M80" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Gauss
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 11
+        flyingThreshold = 200000
+        spaceThreshold = 1250000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>233</v>
+      </c>
+      <c r="B81" t="s">
+        <v>216</v>
+      </c>
+      <c r="C81">
+        <v>6</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I81">
+        <v>12</v>
+      </c>
+      <c r="J81">
+        <v>18000</v>
+      </c>
+      <c r="K81">
+        <v>90000</v>
+      </c>
+      <c r="M81" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Loki
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 90000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" t="s">
+        <v>216</v>
+      </c>
+      <c r="C82">
+        <v>6.5</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="8"/>
+        <v>6.5</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="I82">
+        <v>12</v>
+      </c>
+      <c r="J82">
+        <v>18000</v>
+      </c>
+      <c r="K82">
+        <v>90000</v>
+      </c>
+      <c r="M82" s="1" t="str">
+        <f t="shared" ref="M82:M85" si="12">_xlfn.CONCAT("Item:NEEDS[",B82,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A82,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C82,CHAR(10),"        ",D$1," = ",D82,CHAR(10),"        ",E$1," = ",E82,CHAR(10),"        ",F$1," = ",F82,CHAR(10),"        ",G$1," = ",G82,CHAR(10),"        ",H$1," = ",H82,CHAR(10),"        ",I$1," = ",I82,CHAR(10),"        ",J$1," = ",J82,CHAR(10),"        ",K$1," = ",K82,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Catullus
+    adjustedParams
+    {
+        landedData = 6.5
+        splashedData = 6.5
+        flyingLowData = 5.5
+        flyingHighData = 5.5
+        spaceLowData = 5.5
+        spaceHighData = 5.5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 90000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83">
+        <v>7</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="I83">
+        <v>12</v>
+      </c>
+      <c r="J83">
+        <v>33000</v>
+      </c>
+      <c r="K83">
+        <v>160000</v>
+      </c>
+      <c r="M83" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Tarsiss
+    adjustedParams
+    {
+        landedData = 7
+        splashedData = 7
+        flyingLowData = 6
+        flyingHighData = 6
+        spaceLowData = 6
+        spaceHighData = 6
+        recoveredData = 12
+        flyingThreshold = 33000
+        spaceThreshold = 160000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>236</v>
+      </c>
+      <c r="B84" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84">
+        <v>6</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I84">
+        <v>11</v>
+      </c>
+      <c r="J84">
+        <v>280000</v>
+      </c>
+      <c r="K84">
+        <v>2500000</v>
+      </c>
+      <c r="M84" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Nero
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 11
+        flyingThreshold = 280000
+        spaceThreshold = 2500000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>237</v>
+      </c>
+      <c r="B85" t="s">
+        <v>216</v>
+      </c>
+      <c r="C85">
+        <v>6.5</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="8"/>
+        <v>6.5</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="I85">
+        <v>12</v>
+      </c>
+      <c r="J85">
+        <v>20000</v>
+      </c>
+      <c r="K85">
+        <v>150000</v>
+      </c>
+      <c r="M85" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Hadrian
+    adjustedParams
+    {
+        landedData = 6.5
+        splashedData = 6.5
+        flyingLowData = 5.5
+        flyingHighData = 5.5
+        spaceLowData = 5.5
+        spaceHighData = 5.5
+        recoveredData = 12
+        flyingThreshold = 20000
+        spaceThreshold = 150000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>238</v>
+      </c>
+      <c r="B86" t="s">
+        <v>216</v>
+      </c>
+      <c r="C86">
+        <v>6</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I86">
+        <v>12</v>
+      </c>
+      <c r="J86">
+        <v>18000</v>
+      </c>
+      <c r="K86">
+        <v>45000</v>
+      </c>
+      <c r="M86" s="1" t="str">
+        <f t="shared" ref="M86" si="13">_xlfn.CONCAT("Item:NEEDS[",B86,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A86,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C86,CHAR(10),"        ",D$1," = ",D86,CHAR(10),"        ",E$1," = ",E86,CHAR(10),"        ",F$1," = ",F86,CHAR(10),"        ",G$1," = ",G86,CHAR(10),"        ",H$1," = ",H86,CHAR(10),"        ",I$1," = ",I86,CHAR(10),"        ",J$1," = ",J86,CHAR(10),"        ",K$1," = ",K86,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Narisse
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 45000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>239</v>
+      </c>
+      <c r="B87" t="s">
+        <v>216</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I87">
+        <v>12</v>
+      </c>
+      <c r="J87">
+        <v>18000</v>
+      </c>
+      <c r="K87">
+        <v>65000</v>
+      </c>
+      <c r="M87" s="1" t="str">
+        <f t="shared" ref="M87" si="14">_xlfn.CONCAT("Item:NEEDS[",B87,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A87,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C87,CHAR(10),"        ",D$1," = ",D87,CHAR(10),"        ",E$1," = ",E87,CHAR(10),"        ",F$1," = ",F87,CHAR(10),"        ",G$1," = ",G87,CHAR(10),"        ",H$1," = ",H87,CHAR(10),"        ",I$1," = ",I87,CHAR(10),"        ",J$1," = ",J87,CHAR(10),"        ",K$1," = ",K87,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Muse
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 65000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" t="s">
+        <v>216</v>
+      </c>
+      <c r="C88">
+        <v>6</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>12</v>
+      </c>
+      <c r="J88">
+        <v>18000</v>
+      </c>
+      <c r="K88">
+        <v>60000</v>
+      </c>
+      <c r="M88" s="1" t="str">
+        <f t="shared" ref="M88" si="15">_xlfn.CONCAT("Item:NEEDS[",B88,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A88,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C88,CHAR(10),"        ",D$1," = ",D88,CHAR(10),"        ",E$1," = ",E88,CHAR(10),"        ",F$1," = ",F88,CHAR(10),"        ",G$1," = ",G88,CHAR(10),"        ",H$1," = ",H88,CHAR(10),"        ",I$1," = ",I88,CHAR(10),"        ",J$1," = ",J88,CHAR(10),"        ",K$1," = ",K88,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Minona
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 60000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>241</v>
+      </c>
+      <c r="B89" t="s">
+        <v>216</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I89">
+        <v>12</v>
+      </c>
+      <c r="J89">
+        <v>18000</v>
+      </c>
+      <c r="K89">
+        <v>25000</v>
+      </c>
+      <c r="M89" s="1" t="str">
+        <f t="shared" ref="M89" si="16">_xlfn.CONCAT("Item:NEEDS[",B89,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A89,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C89,CHAR(10),"        ",D$1," = ",D89,CHAR(10),"        ",E$1," = ",E89,CHAR(10),"        ",F$1," = ",F89,CHAR(10),"        ",G$1," = ",G89,CHAR(10),"        ",H$1," = ",H89,CHAR(10),"        ",I$1," = ",I89,CHAR(10),"        ",J$1," = ",J89,CHAR(10),"        ",K$1," = ",K89,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Agrippina
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 18000
+        spaceThreshold = 25000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>242</v>
+      </c>
+      <c r="B90" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90">
+        <v>6</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I90">
+        <v>12</v>
+      </c>
+      <c r="J90">
+        <v>10000</v>
+      </c>
+      <c r="K90">
+        <v>15000</v>
+      </c>
+      <c r="M90" s="1" t="str">
+        <f t="shared" ref="M90:M91" si="17">_xlfn.CONCAT("Item:NEEDS[",B90,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A90,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C90,CHAR(10),"        ",D$1," = ",D90,CHAR(10),"        ",E$1," = ",E90,CHAR(10),"        ",F$1," = ",F90,CHAR(10),"        ",G$1," = ",G90,CHAR(10),"        ",H$1," = ",H90,CHAR(10),"        ",I$1," = ",I90,CHAR(10),"        ",J$1," = ",J90,CHAR(10),"        ",K$1," = ",K90,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Julia
+    adjustedParams
+    {
+        landedData = 6
+        splashedData = 6
+        flyingLowData = 5
+        flyingHighData = 5
+        spaceLowData = 5
+        spaceHighData = 5
+        recoveredData = 12
+        flyingThreshold = 10000
+        spaceThreshold = 15000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>243</v>
+      </c>
+      <c r="B91" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91">
+        <v>7</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="I91">
+        <v>13</v>
+      </c>
+      <c r="J91">
+        <v>10000</v>
+      </c>
+      <c r="K91">
+        <v>125000</v>
+      </c>
+      <c r="M91" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Hox
+    adjustedParams
+    {
+        landedData = 7
+        splashedData = 7
+        flyingLowData = 6
+        flyingHighData = 6
+        spaceLowData = 6
+        spaceHighData = 6
+        recoveredData = 13
+        flyingThreshold = 10000
+        spaceThreshold = 125000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>244</v>
+      </c>
+      <c r="B92" t="s">
+        <v>216</v>
+      </c>
+      <c r="C92">
+        <v>6.5</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="8"/>
+        <v>6.5</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="I92">
+        <v>14</v>
+      </c>
+      <c r="J92">
+        <v>18000</v>
+      </c>
+      <c r="K92">
+        <v>40000</v>
+      </c>
+      <c r="M92" s="1" t="str">
+        <f t="shared" ref="M92:M93" si="18">_xlfn.CONCAT("Item:NEEDS[",B92,"]",CHAR(10),"{",CHAR(10),"    bodyName = ",A92,CHAR(10),"    adjustedParams",CHAR(10),"    {",CHAR(10),"        ",C$1," = ",C92,CHAR(10),"        ",D$1," = ",D92,CHAR(10),"        ",E$1," = ",E92,CHAR(10),"        ",F$1," = ",F92,CHAR(10),"        ",G$1," = ",G92,CHAR(10),"        ",H$1," = ",H92,CHAR(10),"        ",I$1," = ",I92,CHAR(10),"        ",J$1," = ",J92,CHAR(10),"        ",K$1," = ",K92,CHAR(10),"    }",CHAR(10),"}")</f>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Argo
+    adjustedParams
+    {
+        landedData = 6.5
+        splashedData = 6.5
+        flyingLowData = 5.5
+        flyingHighData = 5.5
+        spaceLowData = 5.5
+        spaceHighData = 5.5
+        recoveredData = 14
+        flyingThreshold = 18000
+        spaceThreshold = 40000
+    }
+}</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="232" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>245</v>
+      </c>
+      <c r="B93" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93">
+        <v>7</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="I93">
+        <v>13</v>
+      </c>
+      <c r="J93">
+        <v>9000</v>
+      </c>
+      <c r="K93">
+        <v>105000</v>
+      </c>
+      <c r="M93" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>Item:NEEDS[GPP]
+{
+    bodyName = Leto
+    adjustedParams
+    {
+        landedData = 7
+        splashedData = 7
+        flyingLowData = 6
+        flyingHighData = 6
+        spaceLowData = 6
+        spaceHighData = 6
+        recoveredData = 13
+        flyingThreshold = 9000
+        spaceThreshold = 105000
+    }
+}</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:M68" xr:uid="{AFC65FD1-7BB3-48D7-856F-14AEF5C1B522}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>